<commit_message>
ber skrá saman við rétta lausn og gefur einkunn
</commit_message>
<xml_diff>
--- a/assignment9/hbv205m_assignment09.xlsx
+++ b/assignment9/hbv205m_assignment09.xlsx
@@ -420,7 +420,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -510,6 +510,18 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -782,10 +794,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,9 +909,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,7 +950,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="152400" y="878921"/>
+          <a:off x="152400" y="877981"/>
           <a:ext cx="4676775" cy="3333750"/>
           <a:chOff x="214300" y="535400"/>
           <a:chExt cx="4662400" cy="3311275"/>
@@ -1702,7 +1731,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7338192" y="292100"/>
+          <a:off x="7344522" y="292100"/>
           <a:ext cx="6172200" cy="3952875"/>
           <a:chOff x="357200" y="371300"/>
           <a:chExt cx="6681700" cy="4011450"/>
@@ -2853,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="149" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="136" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3588,8 +3617,8 @@
         <v>16</v>
       </c>
       <c r="J33" s="21"/>
-      <c r="K33" s="18" t="s">
-        <v>15</v>
+      <c r="K33" s="83" t="s">
+        <v>24</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="21"/>
@@ -3613,8 +3642,8 @@
         <v>19</v>
       </c>
       <c r="J34" s="24"/>
-      <c r="K34" s="14" t="s">
-        <v>20</v>
+      <c r="K34" s="84" t="s">
+        <v>25</v>
       </c>
       <c r="M34" s="24"/>
       <c r="W34" s="4"/>
@@ -3627,6 +3656,9 @@
       <c r="A35" s="22"/>
       <c r="I35" s="23"/>
       <c r="J35" s="24"/>
+      <c r="K35" s="84" t="s">
+        <v>27</v>
+      </c>
       <c r="M35" s="24"/>
       <c r="T35" s="4"/>
       <c r="W35" s="4"/>
@@ -3680,7 +3712,7 @@
       </c>
       <c r="J37" s="21"/>
       <c r="K37" s="18" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L37" s="19"/>
       <c r="M37" s="21"/>
@@ -3706,7 +3738,7 @@
       </c>
       <c r="J38" s="24"/>
       <c r="K38" s="14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M38" s="24"/>
       <c r="S38" s="4"/>
@@ -3729,9 +3761,7 @@
         <v>16</v>
       </c>
       <c r="J39" s="24"/>
-      <c r="K39" s="14" t="s">
-        <v>27</v>
-      </c>
+      <c r="K39" s="14"/>
       <c r="M39" s="24"/>
       <c r="Z39" s="4"/>
       <c r="AA39" s="4"/>
@@ -3996,7 +4026,7 @@
     <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="22"/>
       <c r="I50" s="23"/>
-      <c r="K50" s="83"/>
+      <c r="K50" s="14"/>
       <c r="M50" s="24"/>
       <c r="W50" s="4"/>
       <c r="X50" s="4"/>

</xml_diff>